<commit_message>
working on NIDM-Experiment class, Investigation level
</commit_message>
<xml_diff>
--- a/nidm/nidm-experiment/simpledata_example_ohbm_hack_2016/SimpleData.xlsx
+++ b/nidm/nidm-experiment/simpledata_example_ohbm_hack_2016/SimpleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbkeator/Documents/Coding/nidm_experiment_tests/SG_DK_Hackathon_Example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbkeator/Documents/Coding/nidm/nidm/nidm-experiment/simpledata_example_ohbm_hack_2016/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -583,11 +583,13 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>DNK Ubuntu vs. AdamT CentOS</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -632,6 +634,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -747,11 +750,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2102880544"/>
-        <c:axId val="-2102873536"/>
+        <c:axId val="-2111040352"/>
+        <c:axId val="-2111113360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2102880544"/>
+        <c:axId val="-2111040352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,12 +788,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102873536"/>
+        <c:crossAx val="-2111113360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2102873536"/>
+        <c:axId val="-2111113360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,13 +827,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102880544"/>
+        <c:crossAx val="-2111040352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -862,11 +866,13 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>DNK Ubuntu vs. MacOS</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -911,6 +917,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1026,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2102808848"/>
-        <c:axId val="-2102805552"/>
+        <c:axId val="-2111006688"/>
+        <c:axId val="-2111003328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2102808848"/>
+        <c:axId val="-2111006688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,12 +1071,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102805552"/>
+        <c:crossAx val="-2111003328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2102805552"/>
+        <c:axId val="-2111003328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,13 +1110,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102808848"/>
+        <c:crossAx val="-2111006688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1494,9 +1502,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2247,6 +2257,16 @@
       </c>
       <c r="I25" s="4" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C28">
+        <f>AVERAGE(C2:C25)</f>
+        <v>13.5</v>
+      </c>
+      <c r="D28">
+        <f>STDEV(C2:C25)</f>
+        <v>1.4446302370292303</v>
       </c>
     </row>
   </sheetData>
@@ -2470,7 +2490,7 @@
       <c r="Z3" s="15"/>
       <c r="AA3" s="15"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>84</v>
       </c>
@@ -2523,7 +2543,7 @@
         <v>7172808</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>85</v>
       </c>
@@ -2576,7 +2596,7 @@
         <v>6714</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>86</v>
       </c>
@@ -2629,7 +2649,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>87</v>
       </c>
@@ -2682,7 +2702,7 @@
         <v>4087</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>88</v>
       </c>
@@ -2735,7 +2755,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>89</v>
       </c>
@@ -2788,7 +2808,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>90</v>
       </c>
@@ -2841,7 +2861,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>91</v>
       </c>
@@ -2894,7 +2914,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>92</v>
       </c>
@@ -2947,7 +2967,7 @@
         <v>6514</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>93</v>
       </c>
@@ -3000,7 +3020,7 @@
         <v>3064</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>94</v>
       </c>
@@ -3053,7 +3073,7 @@
         <v>3685</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>95</v>
       </c>
@@ -3106,7 +3126,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>96</v>
       </c>
@@ -3159,7 +3179,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>97</v>
       </c>
@@ -3212,7 +3232,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>98</v>
       </c>

</xml_diff>